<commit_message>
Added sums to AHP figures to check some results
</commit_message>
<xml_diff>
--- a/StateOfPractice/Papers/MedImageSoft_SOP-arXiv/figures/AHP_Charts-ForFigures.xlsx
+++ b/StateOfPractice/Papers/MedImageSoft_SOP-arXiv/figures/AHP_Charts-ForFigures.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/AIMSS/StateOfPractice/Papers/MedImageSoft_SOP-arXiv/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FFC361-C557-8D46-A50A-F51F0C1C49C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1BEB2A-8246-E045-B5D4-186C3F51F59C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="1280" windowWidth="37660" windowHeight="24780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="200" yWindow="1280" windowWidth="37660" windowHeight="24780" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="1" r:id="rId1"/>
@@ -7129,8 +7129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8588,7 +8588,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8827,6 +8827,12 @@
       </c>
       <c r="B29" s="2">
         <v>6.5058158528450002E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>1.0000000000000049</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -8852,10 +8858,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9094,6 +9100,12 @@
       </c>
       <c r="B29" s="2">
         <v>7.9604549879210007E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>1.000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -9109,10 +9121,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9351,6 +9363,12 @@
       </c>
       <c r="B29" s="2">
         <v>6.3822513610170004E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>1.0000000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -9366,10 +9384,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9608,6 +9626,12 @@
       </c>
       <c r="B29" s="2">
         <v>5.3304224400590001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>1.0000000000000031</v>
       </c>
     </row>
   </sheetData>
@@ -9623,10 +9647,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9865,6 +9889,12 @@
       </c>
       <c r="B29" s="2">
         <v>5.5512561526279997E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>1.0000000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -9880,10 +9910,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10122,6 +10152,12 @@
       </c>
       <c r="B29" s="2">
         <v>8.6203061140000003E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <f>SUM(B1:B29)</f>
+        <v>0.11111111111111299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>